<commit_message>
Se añadio metodo onGet en el modelo, se añadió detecccion de banco al cargar un pdf y se hizo una actualización de la plantilla y el cardview
</commit_message>
<xml_diff>
--- a/ERPSEI/wwwroot/templates/PlantillaMovimientosBancarios.xlsx
+++ b/ERPSEI/wwwroot/templates/PlantillaMovimientosBancarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Cruz\source\repos\ERPSEI\ERPSEI\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4889F43A-A226-4B38-88E3-BAF0FD1C76D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011349D5-4170-4E7F-AE66-3CBA0E402AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9E524D79-6786-4DAB-8B6C-F7BCDE29EE51}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Fecha</t>
   </si>
@@ -44,7 +44,10 @@
     <t>Descripción</t>
   </si>
   <si>
-    <t>Importe</t>
+    <t>Cargos</t>
+  </si>
+  <si>
+    <t>Abonos</t>
   </si>
 </sst>
 </file>
@@ -82,12 +85,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -96,7 +114,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -433,20 +451,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B1DB96-A029-43D2-A67B-8D3C26845C0B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="66.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,6 +475,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>